<commit_message>
cap nhat BM ViTri KNL
</commit_message>
<xml_diff>
--- a/E-Learning/App_Data/DS_ViTriKNL.xlsx
+++ b/E-Learning/App_Data/DS_ViTriKNL.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hoaphatcomvn-my.sharepoint.com/personal/phuocnv1_hoaphat_com_vn/Documents/Working/Software/KhungNangLuc/production/18112022_v2/Elearning v2/Elearning v2/E-Learning/App_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - hoaphat.com.vn\Working\Software\ELEARNING_DEV\E-Learning\E-Learning\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{2AFC2619-A3A0-440C-A243-F047841B7B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64F6AB6F-BA4B-451F-AC55-ED6231151ED3}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{2AFC2619-A3A0-440C-A243-F047841B7B4F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADBDB2EA-399C-4E90-A956-5A5CB8F87F5A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{60E312A9-B38A-4080-82C8-0F62C17AC0BD}"/>
   </bookViews>
   <sheets>
     <sheet name="DSVT_KNL" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,11 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>STT</t>
   </si>
@@ -65,6 +60,9 @@
   </si>
   <si>
     <t>Mã định danh vị trí KNL</t>
+  </si>
+  <si>
+    <t>Tình trạng hiệu lực Vị trí</t>
   </si>
 </sst>
 </file>
@@ -116,7 +114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -185,35 +183,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -529,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFBD710F-664C-4EDA-B7A0-B52FF52E5DC4}">
-  <dimension ref="A2:I5"/>
+  <dimension ref="A2:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,75 +553,80 @@
     <col min="9" max="9" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="J3" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+    <row r="4" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="9"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="A2:I2"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="A2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>